<commit_message>
FEAT: Chemisty from Richards [2011].
</commit_message>
<xml_diff>
--- a/inputs/chemistry_earth.xlsx
+++ b/inputs/chemistry_earth.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridley/Software/Aether/Aether/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26BFD9B-86A6-1D4A-A370-5D4059BC5053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35B5F74-E4A2-AD4F-BC22-EED457AA785F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20760" yWindow="12120" windowWidth="27240" windowHeight="16440" xr2:uid="{9A327DE2-5707-5C42-9A87-774C409DCA02}"/>
+    <workbookView xWindow="13900" yWindow="3500" windowWidth="27240" windowHeight="18420" xr2:uid="{9A327DE2-5707-5C42-9A87-774C409DCA02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="90">
   <si>
     <t>loss1</t>
   </si>
@@ -106,19 +106,246 @@
   </si>
   <si>
     <t>NO+</t>
+  </si>
+  <si>
+    <t>He+</t>
+  </si>
+  <si>
+    <t>He</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N+</t>
+  </si>
+  <si>
+    <t>Anichich</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O+_2D</t>
+  </si>
+  <si>
+    <t>Bischof and Linder</t>
+  </si>
+  <si>
+    <t>O+_2P</t>
+  </si>
+  <si>
+    <t>O+_4S</t>
+  </si>
+  <si>
+    <t>O_1D</t>
+  </si>
+  <si>
+    <t>Lee at al.</t>
+  </si>
+  <si>
+    <t>1978a,b</t>
+  </si>
+  <si>
+    <t>O_1S</t>
+  </si>
+  <si>
+    <t>Baulch et al</t>
+  </si>
+  <si>
+    <t>Kopp et al</t>
+  </si>
+  <si>
+    <t>Tn*exp(-3270/Tn)</t>
+  </si>
+  <si>
+    <t>(300/Ti)^0.24</t>
+  </si>
+  <si>
+    <t>Fahey et al</t>
+  </si>
+  <si>
+    <t>Anicich</t>
+  </si>
+  <si>
+    <t>Constantinides et al. (1979), Bates (1989)</t>
+  </si>
+  <si>
+    <t>O_3P</t>
+  </si>
+  <si>
+    <t>Dotan et al. (1997), O’Keefe et al. (1986)</t>
+  </si>
+  <si>
+    <t>(300/Te)^0.39</t>
+  </si>
+  <si>
+    <t>Zipf</t>
+  </si>
+  <si>
+    <t>&lt;--- Check with Nagy</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t>Scott et al.</t>
+  </si>
+  <si>
+    <t>(300/Ti)^0.44</t>
+  </si>
+  <si>
+    <t>Ti&lt;=1500</t>
+  </si>
+  <si>
+    <t>(Ti/1500)^0.2</t>
+  </si>
+  <si>
+    <t>Ti&gt;1500</t>
+  </si>
+  <si>
+    <t>(300/Ti)^0.23</t>
+  </si>
+  <si>
+    <t>McFarland et al</t>
+  </si>
+  <si>
+    <t>(300/Ti)^1.16</t>
+  </si>
+  <si>
+    <t>Ti&lt;=1000</t>
+  </si>
+  <si>
+    <t>(Ti/1000)^0.67</t>
+  </si>
+  <si>
+    <t>Ti&gt;1000</t>
+  </si>
+  <si>
+    <t>(300/Te)^0.85</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vejby-Christensen et al. (1998) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>and</t>
+    </r>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>H+</t>
+  </si>
+  <si>
+    <t>Torr and Torr</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>St.-Maurice and Torr (1978), Hierl et al. (1997)</t>
+  </si>
+  <si>
+    <t>(300/Ti)^-0.87</t>
+  </si>
+  <si>
+    <t>Dotan and Viggiano</t>
+  </si>
+  <si>
+    <t>(300/Ti)^0.52</t>
+  </si>
+  <si>
+    <t>Ti&lt;=900</t>
+  </si>
+  <si>
+    <t>(Ti/900)^0.92</t>
+  </si>
+  <si>
+    <t>Ti&gt;900</t>
+  </si>
+  <si>
+    <t>(300/Te)^0.70</t>
+  </si>
+  <si>
+    <t>Ti&lt;=1200</t>
+  </si>
+  <si>
+    <t>Ti&gt;1200</t>
+  </si>
+  <si>
+    <t>(1200/Te)^0.56</t>
+  </si>
+  <si>
+    <t>&lt;--- Ti or Ti???</t>
+  </si>
+  <si>
+    <t>Mehr and Biondi</t>
+  </si>
+  <si>
+    <t>N(2D)</t>
+  </si>
+  <si>
+    <t>Goldan</t>
+  </si>
+  <si>
+    <t>O'Keefe</t>
+  </si>
+  <si>
+    <t>&lt;--- doesn't balance!</t>
+  </si>
+  <si>
+    <t>N_2P</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Midey and Viggiano</t>
+  </si>
+  <si>
+    <t>(300/Ti)^0.45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000066"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,10 +368,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,15 +689,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61AEBFE-9942-424C-99F8-6F883E60C25B}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,14 +725,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -524,104 +757,1111 @@
       <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <f>0.000000000000195*0.43</f>
-        <v>8.3850000000000004E-14</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.3860000000000001E-13</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="2">
-        <v>1.3860000000000001E-13</v>
-      </c>
-      <c r="I4">
-        <v>0.44</v>
-      </c>
-      <c r="J4">
-        <v>5.77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1.2E-18</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
       <c r="H5" s="2">
-        <v>1.3860000000000001E-13</v>
-      </c>
-      <c r="I5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J5">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>7.7999999999999995E-16</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5.1999999999999997E-16</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.35E-15</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2">
+        <v>9.9999999999999998E-17</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.3700000000000001E-16</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.0400000000000005E-17</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2.3900000000000001E-17</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.6000000000000002E-17</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2">
+        <v>9.2000000000000004E-18</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3.3999999999999998E-17</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="O14" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.5000000000000001E-20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2.4999999999999999E-17</v>
+      </c>
+      <c r="O16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8.3300000000000005E-17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P17">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F18" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2">
-        <v>1.2E-18</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1.1000000000000001</v>
+      <c r="H18" s="2">
+        <v>4.7199999999999998E-16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2.1999999999999998E-18</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.4999999999999996E-16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20">
+        <v>0.36</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H21" s="2">
+        <v>9.5000000000000005E-16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5.4999999999999996E-16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H23" s="2">
+        <v>9.5000000000000005E-16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5.4999999999999996E-16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H25" s="2">
+        <v>9.5000000000000005E-16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2">
+        <v>5.4999999999999996E-16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H27" s="2">
+        <v>9.5000000000000005E-16</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5.4999999999999996E-16</v>
+      </c>
+      <c r="I28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H29" s="2">
+        <v>9.5000000000000005E-16</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.2E-13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>48</v>
+      </c>
+      <c r="O30" t="s">
+        <v>49</v>
+      </c>
+      <c r="P30">
+        <v>1980</v>
+      </c>
+      <c r="R30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.1E-17</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="P31">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="2">
+        <v>3.5999999999999998E-16</v>
+      </c>
+      <c r="O32" t="s">
+        <v>52</v>
+      </c>
+      <c r="P32">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.3299999999999999E-16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>53</v>
+      </c>
+      <c r="J33" t="s">
+        <v>54</v>
+      </c>
+      <c r="O33" t="s">
+        <v>52</v>
+      </c>
+      <c r="P33">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H34" s="2">
+        <v>6.5500000000000004E-17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6.9999999999999997E-18</v>
+      </c>
+      <c r="I35" t="s">
+        <v>57</v>
+      </c>
+      <c r="O35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="2">
+        <v>5.1000000000000003E-17</v>
+      </c>
+      <c r="I36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" t="s">
+        <v>60</v>
+      </c>
+      <c r="O36" t="s">
+        <v>52</v>
+      </c>
+      <c r="P36">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H37" s="2">
+        <v>1.2600000000000001E-17</v>
+      </c>
+      <c r="I37" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2">
+        <v>3.4000000000000002E-13</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="2">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="I39" t="s">
+        <v>63</v>
+      </c>
+      <c r="O39" t="s">
+        <v>67</v>
+      </c>
+      <c r="P39">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="2">
+        <v>6.4000000000000005E-16</v>
+      </c>
+      <c r="O40" t="s">
+        <v>44</v>
+      </c>
+      <c r="P40">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1.2999999999999999E-16</v>
+      </c>
+      <c r="O41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>68</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="2">
+        <v>7.0000000000000003E-19</v>
+      </c>
+      <c r="I43" t="s">
+        <v>70</v>
+      </c>
+      <c r="O43" t="s">
+        <v>71</v>
+      </c>
+      <c r="P43">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1.6000000000000001E-17</v>
+      </c>
+      <c r="I44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H45" s="2">
+        <v>8.9999999999999999E-18</v>
+      </c>
+      <c r="I45" t="s">
+        <v>74</v>
+      </c>
+      <c r="J45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1.95E-13</v>
+      </c>
+      <c r="I46" t="s">
+        <v>76</v>
+      </c>
+      <c r="J46" t="s">
+        <v>77</v>
+      </c>
+      <c r="O46" t="s">
+        <v>81</v>
+      </c>
+      <c r="P46">
+        <v>1969</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H47" s="2">
+        <v>7.3900000000000006E-14</v>
+      </c>
+      <c r="I47" t="s">
+        <v>79</v>
+      </c>
+      <c r="J47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="2">
+        <v>1.7999999999999999E-16</v>
+      </c>
+      <c r="O48" t="s">
+        <v>83</v>
+      </c>
+      <c r="P48">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="2">
+        <v>8.65E-17</v>
+      </c>
+      <c r="O49" t="s">
+        <v>84</v>
+      </c>
+      <c r="P49">
+        <v>1986</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="2">
+        <v>2.1999999999999998E-18</v>
+      </c>
+      <c r="O50" t="s">
+        <v>49</v>
+      </c>
+      <c r="P50">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="2">
+        <v>9.9999999999999998E-17</v>
+      </c>
+      <c r="O51" t="s">
+        <v>87</v>
+      </c>
+      <c r="P51">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="2">
+        <v>4.5000000000000002E-16</v>
+      </c>
+      <c r="O52" t="s">
+        <v>88</v>
+      </c>
+      <c r="P52">
+        <v>1999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>